<commit_message>
add notes 2 TC
</commit_message>
<xml_diff>
--- a/API_Test_Data/API_Test_Data_Excel.xlsx
+++ b/API_Test_Data/API_Test_Data_Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Test_Data" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="403">
   <si>
     <t>Password</t>
   </si>
@@ -1247,6 +1247,12 @@
   </si>
   <si>
     <t>65437a182a20514fe0422a27</t>
+  </si>
+  <si>
+    <t>CaseId</t>
+  </si>
+  <si>
+    <t>65437535263a4d61e9244be1</t>
   </si>
 </sst>
 </file>
@@ -1881,6 +1887,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1941,7 +1948,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2259,7 +2265,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -2279,7 +2285,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -2297,7 +2303,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
+      <c r="A4" s="87"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
@@ -2315,7 +2321,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -2333,7 +2339,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="87"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -2433,7 +2439,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
         <v>210</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2492,7 +2498,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="92"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="46"/>
       <c r="C3" s="21" t="s">
         <v>211</v>
@@ -2545,7 +2551,7 @@
       <c r="S3" s="21"/>
     </row>
     <row r="4" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="92"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -2600,7 +2606,7 @@
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21" t="s">
         <v>195</v>
@@ -2625,7 +2631,7 @@
       <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -2652,7 +2658,7 @@
       <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21" t="s">
         <v>235</v>
@@ -2677,7 +2683,7 @@
       <c r="S7" s="21"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="8" t="s">
         <v>151</v>
       </c>
@@ -2704,7 +2710,7 @@
       <c r="S8" s="17"/>
     </row>
     <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21" t="s">
         <v>216</v>
@@ -2737,7 +2743,7 @@
       <c r="S9" s="21"/>
     </row>
     <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="92"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="9" t="s">
         <v>158</v>
       </c>
@@ -2772,7 +2778,7 @@
       <c r="S10" s="17"/>
     </row>
     <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
+      <c r="A11" s="93"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21" t="s">
         <v>271</v>
@@ -2799,7 +2805,7 @@
       <c r="S11" s="21"/>
     </row>
     <row r="12" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="92"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="8" t="s">
         <v>69</v>
       </c>
@@ -2828,7 +2834,7 @@
       <c r="S12" s="17"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="92"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>196</v>
@@ -2859,7 +2865,7 @@
       <c r="S13" s="21"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
+      <c r="A14" s="94"/>
       <c r="B14" s="8" t="s">
         <v>275</v>
       </c>
@@ -2935,7 +2941,7 @@
       <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>285</v>
       </c>
       <c r="B2" s="52" t="s">
@@ -2953,7 +2959,7 @@
       <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="52" t="s">
         <v>10</v>
       </c>
@@ -2969,7 +2975,7 @@
       <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="97"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="56" t="s">
         <v>282</v>
       </c>
@@ -2987,7 +2993,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="98"/>
+      <c r="A5" s="99"/>
       <c r="B5" s="52" t="s">
         <v>11</v>
       </c>
@@ -3178,7 +3184,7 @@
       <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
+      <c r="A3" s="100"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
         <v>216</v>
@@ -3202,7 +3208,7 @@
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="61" t="s">
         <v>10</v>
       </c>
@@ -3276,7 +3282,7 @@
       <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="102" t="s">
         <v>321</v>
       </c>
       <c r="B7" s="21"/>
@@ -3302,7 +3308,7 @@
       <c r="J7" s="25"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
+      <c r="A8" s="103"/>
       <c r="B8" s="17" t="s">
         <v>151</v>
       </c>
@@ -3373,7 +3379,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -3432,7 +3438,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="104"/>
+      <c r="A2" s="105"/>
       <c r="C2" t="s">
         <v>307</v>
       </c>
@@ -3756,7 +3762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -5178,7 +5184,7 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5264,7 +5270,7 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -5344,7 +5350,7 @@
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
@@ -5424,7 +5430,7 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -5504,7 +5510,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="21" t="s">
         <v>1</v>
       </c>
@@ -5579,7 +5585,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="28" t="s">
         <v>151</v>
       </c>
@@ -5652,7 +5658,7 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="21" t="s">
         <v>1</v>
       </c>
@@ -5757,7 +5763,7 @@
       </c>
     </row>
     <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="88"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="8" t="s">
         <v>152</v>
       </c>
@@ -5814,7 +5820,7 @@
       <c r="AI9" s="17"/>
     </row>
     <row r="10" spans="1:35" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="21" t="s">
         <v>1</v>
       </c>
@@ -5904,7 +5910,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="8" t="s">
         <v>153</v>
       </c>
@@ -5992,7 +5998,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="21" t="s">
         <v>1</v>
       </c>
@@ -6036,7 +6042,7 @@
       <c r="AD12" s="38"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="8" t="s">
         <v>158</v>
       </c>
@@ -6080,7 +6086,7 @@
       <c r="AD13" s="38"/>
     </row>
     <row r="14" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="21" t="s">
         <v>1</v>
       </c>
@@ -6185,7 +6191,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
+      <c r="A15" s="89"/>
       <c r="B15" s="8" t="s">
         <v>69</v>
       </c>
@@ -6268,10 +6274,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6281,7 +6287,7 @@
     <col min="10" max="10" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>6</v>
       </c>
@@ -6313,8 +6319,59 @@
         <v>263</v>
       </c>
       <c r="K1" s="84"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -6324,10 +6381,10 @@
       <c r="D2">
         <v>30</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="85" t="s">
         <v>396</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="F2" s="85" t="s">
         <v>399</v>
       </c>
       <c r="G2">
@@ -6342,8 +6399,59 @@
       <c r="J2" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="U2" s="9">
+        <v>7000</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -6353,10 +6461,10 @@
       <c r="D3">
         <v>30</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="85" t="s">
         <v>396</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="85" t="s">
         <v>399</v>
       </c>
       <c r="G3">
@@ -6482,7 +6590,7 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="90" t="s">
         <v>257</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -6550,7 +6658,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="90"/>
+      <c r="A3" s="91"/>
       <c r="B3" s="8"/>
       <c r="C3" s="35" t="s">
         <v>195</v>
@@ -6578,7 +6686,7 @@
       <c r="V3" s="17"/>
     </row>
     <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="90"/>
+      <c r="A4" s="91"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
@@ -6608,7 +6716,7 @@
       <c r="V4" s="17"/>
     </row>
     <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="90"/>
+      <c r="A5" s="91"/>
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -6640,7 +6748,7 @@
       <c r="V5" s="17"/>
     </row>
     <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="90"/>
+      <c r="A6" s="91"/>
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
@@ -6672,7 +6780,7 @@
       <c r="V6" s="17"/>
     </row>
     <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="90"/>
+      <c r="A7" s="91"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -6728,7 +6836,7 @@
       <c r="V7" s="17"/>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="90"/>
+      <c r="A8" s="91"/>
       <c r="B8" s="14" t="s">
         <v>151</v>
       </c>
@@ -7050,7 +7158,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -7139,7 +7247,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A3" s="92"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="52" t="s">
         <v>10</v>
       </c>
@@ -7226,7 +7334,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="92"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="52" t="s">
         <v>11</v>
       </c>
@@ -7313,7 +7421,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="93"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
@@ -7409,7 +7517,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>149</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -7426,7 +7534,7 @@
       <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -7459,13 +7567,13 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="95"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -7642,7 +7750,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>201</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -7668,7 +7776,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
@@ -7690,7 +7798,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -7712,7 +7820,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
@@ -7734,7 +7842,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="21" t="s">
         <v>1</v>
       </c>
@@ -7750,7 +7858,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="8" t="s">
         <v>151</v>
       </c>
@@ -7766,7 +7874,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="8" t="s">
         <v>152</v>
       </c>
@@ -7782,7 +7890,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -7792,7 +7900,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -7844,7 +7952,7 @@
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>209</v>
       </c>
       <c r="B2" s="8"/>
@@ -7856,7 +7964,7 @@
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -7866,7 +7974,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
@@ -7876,7 +7984,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="41"/>
@@ -7886,7 +7994,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -7896,7 +8004,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="8"/>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
@@ -7906,7 +8014,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="8"/>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -7916,7 +8024,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -7926,7 +8034,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -7978,7 +8086,7 @@
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>210</v>
       </c>
       <c r="B2" s="8"/>
@@ -7990,7 +8098,7 @@
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -8000,7 +8108,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
@@ -8010,7 +8118,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="41"/>
@@ -8020,7 +8128,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -8030,7 +8138,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="8"/>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
@@ -8040,7 +8148,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="8"/>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -8050,7 +8158,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -8060,7 +8168,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>

</xml_diff>

<commit_message>
vs test data edit
</commit_message>
<xml_diff>
--- a/API_Test_Data/API_Test_Data_Excel.xlsx
+++ b/API_Test_Data/API_Test_Data_Excel.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Hub\FF_Automation_Script_13_09_2023\API_Test_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0C0351-3F73-4412-AB4C-FE7AC95D169C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Test_Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +25,7 @@
     <sheet name="Visitor_Search_Test_Data" sheetId="16" r:id="rId16"/>
     <sheet name="Enrollment_Data_Test_Data" sheetId="17" r:id="rId17"/>
     <sheet name="Integration_Test_Data" sheetId="19" r:id="rId18"/>
-    <sheet name="Integration_VS_Metada_Test_Data" sheetId="20" r:id="rId19"/>
+    <sheet name="Integration_VS_Test_Data" sheetId="20" r:id="rId19"/>
     <sheet name="Approve_enrollment_test_data" sheetId="21" r:id="rId20"/>
     <sheet name="Disable_enrollment_test_data" sheetId="22" r:id="rId21"/>
   </sheets>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="424">
   <si>
     <t>Password</t>
   </si>
@@ -1239,9 +1233,6 @@
     <t>CaseId</t>
   </si>
   <si>
-    <t>65437535263a4d61e9244be1</t>
-  </si>
-  <si>
     <t>Create_User_Test_Data</t>
   </si>
   <si>
@@ -1300,12 +1291,27 @@
   </si>
   <si>
     <t>INT_01_Disable_EN_EG</t>
+  </si>
+  <si>
+    <t>API_Name</t>
+  </si>
+  <si>
+    <t>Start Search</t>
+  </si>
+  <si>
+    <t>create enrollment</t>
+  </si>
+  <si>
+    <t>add_notes</t>
+  </si>
+  <si>
+    <t>enrollment index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1729,7 +1735,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1943,7 +1949,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2019,6 +2024,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2292,14 +2305,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2336,7 +2349,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="85" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -2356,7 +2369,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="87"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -2374,7 +2387,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
@@ -2392,7 +2405,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="87"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -2410,7 +2423,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="88"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -2434,7 +2447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2510,7 +2523,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="91" t="s">
         <v>210</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2569,7 +2582,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="93"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="46"/>
       <c r="C3" s="21" t="s">
         <v>211</v>
@@ -2622,7 +2635,7 @@
       <c r="S3" s="21"/>
     </row>
     <row r="4" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="93"/>
+      <c r="A4" s="92"/>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -2677,7 +2690,7 @@
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="93"/>
+      <c r="A5" s="92"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21" t="s">
         <v>195</v>
@@ -2702,7 +2715,7 @@
       <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="93"/>
+      <c r="A6" s="92"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -2729,7 +2742,7 @@
       <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="93"/>
+      <c r="A7" s="92"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21" t="s">
         <v>235</v>
@@ -2754,7 +2767,7 @@
       <c r="S7" s="21"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="93"/>
+      <c r="A8" s="92"/>
       <c r="B8" s="8" t="s">
         <v>151</v>
       </c>
@@ -2781,7 +2794,7 @@
       <c r="S8" s="17"/>
     </row>
     <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="93"/>
+      <c r="A9" s="92"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21" t="s">
         <v>216</v>
@@ -2814,7 +2827,7 @@
       <c r="S9" s="21"/>
     </row>
     <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="93"/>
+      <c r="A10" s="92"/>
       <c r="B10" s="9" t="s">
         <v>158</v>
       </c>
@@ -2849,7 +2862,7 @@
       <c r="S10" s="17"/>
     </row>
     <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="93"/>
+      <c r="A11" s="92"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21" t="s">
         <v>271</v>
@@ -2876,7 +2889,7 @@
       <c r="S11" s="21"/>
     </row>
     <row r="12" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="93"/>
+      <c r="A12" s="92"/>
       <c r="B12" s="8" t="s">
         <v>69</v>
       </c>
@@ -2905,7 +2918,7 @@
       <c r="S12" s="17"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="93"/>
+      <c r="A13" s="92"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>196</v>
@@ -2936,7 +2949,7 @@
       <c r="S13" s="21"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="94"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="8" t="s">
         <v>275</v>
       </c>
@@ -2978,7 +2991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3012,7 +3025,7 @@
       <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="96" t="s">
         <v>285</v>
       </c>
       <c r="B2" s="52" t="s">
@@ -3030,7 +3043,7 @@
       <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="98"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="52" t="s">
         <v>10</v>
       </c>
@@ -3046,7 +3059,7 @@
       <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="98"/>
+      <c r="A4" s="97"/>
       <c r="B4" s="56" t="s">
         <v>282</v>
       </c>
@@ -3064,7 +3077,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="52" t="s">
         <v>11</v>
       </c>
@@ -3090,7 +3103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3160,7 +3173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3193,7 +3206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3255,7 +3268,7 @@
       <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
+      <c r="A3" s="99"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
         <v>216</v>
@@ -3279,7 +3292,7 @@
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="101"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="61" t="s">
         <v>10</v>
       </c>
@@ -3353,7 +3366,7 @@
       <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="101" t="s">
         <v>321</v>
       </c>
       <c r="B7" s="21"/>
@@ -3379,7 +3392,7 @@
       <c r="J7" s="25"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="103"/>
+      <c r="A8" s="102"/>
       <c r="B8" s="17" t="s">
         <v>151</v>
       </c>
@@ -3435,7 +3448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3450,7 +3463,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="103" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -3509,7 +3522,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="105"/>
+      <c r="A2" s="104"/>
       <c r="C2" t="s">
         <v>307</v>
       </c>
@@ -3549,14 +3562,14 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3765,7 +3778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3779,10 +3792,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -5059,39 +5072,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AR2" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
-    <hyperlink ref="AS2" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
-    <hyperlink ref="AR3" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
-    <hyperlink ref="AS3" r:id="rId4" xr:uid="{00000000-0004-0000-1200-000003000000}"/>
-    <hyperlink ref="AR4" r:id="rId5" xr:uid="{00000000-0004-0000-1200-000004000000}"/>
-    <hyperlink ref="AS4" r:id="rId6" xr:uid="{00000000-0004-0000-1200-000005000000}"/>
-    <hyperlink ref="AR5" r:id="rId7" xr:uid="{00000000-0004-0000-1200-000006000000}"/>
-    <hyperlink ref="AS5" r:id="rId8" xr:uid="{00000000-0004-0000-1200-000007000000}"/>
-    <hyperlink ref="AR6" r:id="rId9" xr:uid="{00000000-0004-0000-1200-000008000000}"/>
-    <hyperlink ref="AS6" r:id="rId10" xr:uid="{00000000-0004-0000-1200-000009000000}"/>
+    <hyperlink ref="AR2" r:id="rId1"/>
+    <hyperlink ref="AS2" r:id="rId2"/>
+    <hyperlink ref="AR3" r:id="rId3"/>
+    <hyperlink ref="AS3" r:id="rId4"/>
+    <hyperlink ref="AR4" r:id="rId5"/>
+    <hyperlink ref="AS4" r:id="rId6"/>
+    <hyperlink ref="AR5" r:id="rId7"/>
+    <hyperlink ref="AS5" r:id="rId8"/>
+    <hyperlink ref="AR6" r:id="rId9"/>
+    <hyperlink ref="AS6" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="20.21875" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
     <col min="10" max="10" width="25.21875" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="32" max="32" width="13.88671875" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" customWidth="1"/>
+    <col min="53" max="53" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>6</v>
+        <v>419</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
@@ -5100,187 +5119,685 @@
         <v>338</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>339</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>340</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>344</v>
-      </c>
-      <c r="H1" s="81" t="s">
-        <v>343</v>
-      </c>
-      <c r="I1" s="81" t="s">
-        <v>394</v>
-      </c>
-      <c r="J1" s="81" t="s">
         <v>263</v>
       </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="82"/>
       <c r="L1" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH1" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="AI1" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AU1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AV1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AY1" s="21" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="BA1" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="BD1" s="40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>420</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="110">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="9">
+        <v>1</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="V2" s="17">
+        <v>1</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC2" s="17">
+        <v>5000</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF2" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="AH2" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AR2" s="9">
+        <v>7000</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AU2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="BB2" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="9">
+        <v>100</v>
+      </c>
+      <c r="BD2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="36"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="H3" s="81" t="s">
+        <v>343</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>394</v>
+      </c>
+      <c r="J3" s="81" t="s">
+        <v>263</v>
+      </c>
+      <c r="K3" s="82"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+    </row>
+    <row r="4" spans="1:56" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C4" s="17">
         <v>0.25</v>
       </c>
-      <c r="D2">
+      <c r="D4" s="17">
         <v>30</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E4" s="108" t="s">
         <v>393</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F4" s="108" t="s">
         <v>396</v>
       </c>
-      <c r="G2">
+      <c r="G4" s="17">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H4" s="17">
         <v>50</v>
       </c>
-      <c r="I2" t="b">
+      <c r="I4" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J4" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L4" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="V4" s="17">
+        <v>1</v>
+      </c>
+      <c r="W4" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="X4" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y4" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z4" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB4" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC4" s="17">
+        <v>5000</v>
+      </c>
+      <c r="AD4" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE4" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF4" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="AH4" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="AK4" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="AL4" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="AM4" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="AN4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="AO4" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="AP4" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="AQ4" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="U2" s="9">
+      <c r="AR4" s="9">
         <v>7000</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="AS4" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="AT4" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="AU4" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="AV4" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="Z2" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AW4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AB2" s="9" t="b">
+      <c r="AX4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY4" s="9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="BA4" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="BB4" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="9">
+        <v>100</v>
+      </c>
+      <c r="BD4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="17">
         <v>0.25</v>
       </c>
-      <c r="D3">
+      <c r="D5" s="17">
         <v>30</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E5" s="108" t="s">
         <v>393</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F5" s="108" t="s">
         <v>396</v>
       </c>
-      <c r="G3">
+      <c r="G5" s="17">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="H5" s="17">
         <v>50</v>
       </c>
-      <c r="I3" t="b">
+      <c r="I5" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J5" s="17" t="s">
         <v>397</v>
       </c>
+      <c r="L5" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="V5" s="17">
+        <v>1</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="X5" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z5" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB5" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC5" s="17">
+        <v>5000</v>
+      </c>
+      <c r="AD5" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE5" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF5" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="AH5" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO5" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ5" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AR5" s="9">
+        <v>7000</v>
+      </c>
+      <c r="AS5" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT5" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AU5" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV5" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA5" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="BB5" s="8">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="9">
+        <v>100</v>
+      </c>
+      <c r="BD5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="111"/>
+      <c r="T6" s="111"/>
+      <c r="U6" s="111"/>
+      <c r="V6" s="111"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="111"/>
+      <c r="Y6" s="111"/>
+      <c r="Z6" s="111"/>
+      <c r="AA6" s="111"/>
+      <c r="AB6" s="111"/>
+      <c r="AC6" s="111"/>
+      <c r="AD6" s="111"/>
+      <c r="AE6" s="111"/>
+      <c r="AF6" s="111"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5289,7 +5806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5418,7 +5935,7 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="88" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5504,7 +6021,7 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -5584,7 +6101,7 @@
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
@@ -5664,7 +6181,7 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -5744,7 +6261,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="21" t="s">
         <v>1</v>
       </c>
@@ -5819,7 +6336,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="28" t="s">
         <v>151</v>
       </c>
@@ -5892,7 +6409,7 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
+      <c r="A8" s="88"/>
       <c r="B8" s="21" t="s">
         <v>1</v>
       </c>
@@ -5997,7 +6514,7 @@
       </c>
     </row>
     <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="89"/>
+      <c r="A9" s="88"/>
       <c r="B9" s="8" t="s">
         <v>152</v>
       </c>
@@ -6054,7 +6571,7 @@
       <c r="AI9" s="17"/>
     </row>
     <row r="10" spans="1:35" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="21" t="s">
         <v>1</v>
       </c>
@@ -6144,7 +6661,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
+      <c r="A11" s="88"/>
       <c r="B11" s="8" t="s">
         <v>153</v>
       </c>
@@ -6232,7 +6749,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="89"/>
+      <c r="A12" s="88"/>
       <c r="B12" s="21" t="s">
         <v>1</v>
       </c>
@@ -6276,7 +6793,7 @@
       <c r="AD12" s="38"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
+      <c r="A13" s="88"/>
       <c r="B13" s="8" t="s">
         <v>158</v>
       </c>
@@ -6320,7 +6837,7 @@
       <c r="AD13" s="38"/>
     </row>
     <row r="14" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="89"/>
+      <c r="A14" s="88"/>
       <c r="B14" s="21" t="s">
         <v>1</v>
       </c>
@@ -6425,7 +6942,7 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="89"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="8" t="s">
         <v>69</v>
       </c>
@@ -6484,30 +7001,30 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="P3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="Q3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="P4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Q4" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="P5" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="Q5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="P11" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="Q11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="L9" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="T9" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="AE15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="AF15" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="AG15" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="P3" r:id="rId3"/>
+    <hyperlink ref="Q3" r:id="rId4"/>
+    <hyperlink ref="P4" r:id="rId5"/>
+    <hyperlink ref="Q4" r:id="rId6"/>
+    <hyperlink ref="P5" r:id="rId7"/>
+    <hyperlink ref="Q5" r:id="rId8"/>
+    <hyperlink ref="P11" r:id="rId9"/>
+    <hyperlink ref="Q11" r:id="rId10"/>
+    <hyperlink ref="F9" r:id="rId11"/>
+    <hyperlink ref="L9" r:id="rId12"/>
+    <hyperlink ref="T9" r:id="rId13"/>
+    <hyperlink ref="AE15" r:id="rId14"/>
+    <hyperlink ref="AF15" r:id="rId15"/>
+    <hyperlink ref="AG15" r:id="rId16"/>
+    <hyperlink ref="F13" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6517,7 +7034,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:103" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="83" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -6604,8 +7121,8 @@
       <c r="AC1" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="AD1" s="106" t="s">
-        <v>400</v>
+      <c r="AD1" s="105" t="s">
+        <v>399</v>
       </c>
       <c r="AE1" s="12" t="s">
         <v>17</v>
@@ -6685,8 +7202,8 @@
       <c r="BD1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BE1" s="106" t="s">
-        <v>401</v>
+      <c r="BE1" s="105" t="s">
+        <v>400</v>
       </c>
       <c r="BF1" s="21" t="s">
         <v>138</v>
@@ -6706,8 +7223,8 @@
       <c r="BK1" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="BL1" s="106" t="s">
-        <v>402</v>
+      <c r="BL1" s="105" t="s">
+        <v>401</v>
       </c>
       <c r="BM1" s="35" t="s">
         <v>138</v>
@@ -6736,8 +7253,8 @@
       <c r="BU1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="BV1" s="108" t="s">
-        <v>403</v>
+      <c r="BV1" s="107" t="s">
+        <v>402</v>
       </c>
       <c r="BW1" s="12" t="s">
         <v>163</v>
@@ -6803,36 +7320,36 @@
         <v>239</v>
       </c>
       <c r="CS1" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="CT1" s="21" t="s">
         <v>244</v>
       </c>
       <c r="CU1" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="CV1" s="21" t="s">
         <v>359</v>
       </c>
       <c r="CW1" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="CX1" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="CY1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:103" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="84" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="2" spans="1:103" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
-        <v>409</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>362</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
@@ -6912,7 +7429,7 @@
       <c r="AC2" s="9">
         <v>15</v>
       </c>
-      <c r="AD2" s="107"/>
+      <c r="AD2" s="106"/>
       <c r="AE2" s="9" t="s">
         <v>13</v>
       </c>
@@ -6986,17 +7503,17 @@
         <v>395</v>
       </c>
       <c r="BC2" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="BD2" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="BE2" s="107"/>
+      <c r="BE2" s="106"/>
       <c r="BF2" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="BG2" s="9" t="s">
         <v>412</v>
-      </c>
-      <c r="BG2" s="9" t="s">
-        <v>413</v>
       </c>
       <c r="BH2" s="9" t="s">
         <v>203</v>
@@ -7010,12 +7527,12 @@
       <c r="BK2" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="BL2" s="107"/>
+      <c r="BL2" s="106"/>
       <c r="BM2" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="BN2" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="BO2" s="9">
         <v>0.83</v>
@@ -7038,7 +7555,7 @@
       <c r="BU2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="BV2" s="108"/>
+      <c r="BV2" s="107"/>
       <c r="BW2" s="23" t="s">
         <v>59</v>
       </c>
@@ -7131,15 +7648,15 @@
     <mergeCell ref="BV1:BV2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AR2" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="AS2" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="AR2" r:id="rId1"/>
+    <hyperlink ref="AS2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7149,7 +7666,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:103" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="83" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -7236,8 +7753,8 @@
       <c r="AC1" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="AD1" s="106" t="s">
-        <v>400</v>
+      <c r="AD1" s="105" t="s">
+        <v>399</v>
       </c>
       <c r="AE1" s="12" t="s">
         <v>17</v>
@@ -7317,8 +7834,8 @@
       <c r="BD1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BE1" s="106" t="s">
-        <v>401</v>
+      <c r="BE1" s="105" t="s">
+        <v>400</v>
       </c>
       <c r="BF1" s="21" t="s">
         <v>138</v>
@@ -7338,8 +7855,8 @@
       <c r="BK1" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="BL1" s="106" t="s">
-        <v>402</v>
+      <c r="BL1" s="105" t="s">
+        <v>401</v>
       </c>
       <c r="BM1" s="35" t="s">
         <v>138</v>
@@ -7368,8 +7885,8 @@
       <c r="BU1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="BV1" s="108" t="s">
-        <v>403</v>
+      <c r="BV1" s="107" t="s">
+        <v>402</v>
       </c>
       <c r="BW1" s="12" t="s">
         <v>163</v>
@@ -7435,36 +7952,36 @@
         <v>239</v>
       </c>
       <c r="CS1" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="CT1" s="21" t="s">
         <v>244</v>
       </c>
       <c r="CU1" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="CV1" s="21" t="s">
         <v>359</v>
       </c>
       <c r="CW1" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="CX1" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="CY1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:103" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="84" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="2" spans="1:103" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
-        <v>409</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>362</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
@@ -7544,7 +8061,7 @@
       <c r="AC2" s="9">
         <v>15</v>
       </c>
-      <c r="AD2" s="107"/>
+      <c r="AD2" s="106"/>
       <c r="AE2" s="9" t="s">
         <v>13</v>
       </c>
@@ -7618,17 +8135,17 @@
         <v>395</v>
       </c>
       <c r="BC2" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BD2" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="BE2" s="107"/>
+      <c r="BE2" s="106"/>
       <c r="BF2" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="BG2" s="9" t="s">
         <v>417</v>
-      </c>
-      <c r="BG2" s="9" t="s">
-        <v>418</v>
       </c>
       <c r="BH2" s="9" t="s">
         <v>203</v>
@@ -7642,12 +8159,12 @@
       <c r="BK2" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="BL2" s="107"/>
+      <c r="BL2" s="106"/>
       <c r="BM2" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="BN2" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="BO2" s="9">
         <v>0.83</v>
@@ -7670,7 +8187,7 @@
       <c r="BU2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="BV2" s="108"/>
+      <c r="BV2" s="107"/>
       <c r="BW2" s="23" t="s">
         <v>59</v>
       </c>
@@ -7763,19 +8280,19 @@
     <mergeCell ref="BV1:BV2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AR2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="AS2" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
+    <hyperlink ref="AR2" r:id="rId1"/>
+    <hyperlink ref="AS2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7874,7 +8391,7 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>257</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -7942,7 +8459,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="91"/>
+      <c r="A3" s="90"/>
       <c r="B3" s="8"/>
       <c r="C3" s="35" t="s">
         <v>195</v>
@@ -7970,7 +8487,7 @@
       <c r="V3" s="17"/>
     </row>
     <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="91"/>
+      <c r="A4" s="90"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
@@ -8000,7 +8517,7 @@
       <c r="V4" s="17"/>
     </row>
     <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="91"/>
+      <c r="A5" s="90"/>
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -8032,7 +8549,7 @@
       <c r="V5" s="17"/>
     </row>
     <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91"/>
+      <c r="A6" s="90"/>
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
@@ -8064,7 +8581,7 @@
       <c r="V6" s="17"/>
     </row>
     <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="91"/>
+      <c r="A7" s="90"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -8120,7 +8637,7 @@
       <c r="V7" s="17"/>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="91"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="14" t="s">
         <v>151</v>
       </c>
@@ -8327,7 +8844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8442,7 +8959,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="91" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -8531,7 +9048,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A3" s="93"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="52" t="s">
         <v>10</v>
       </c>
@@ -8618,7 +9135,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="93"/>
+      <c r="A4" s="92"/>
       <c r="B4" s="52" t="s">
         <v>11</v>
       </c>
@@ -8705,7 +9222,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
@@ -8744,7 +9261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
@@ -8801,7 +9318,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="94" t="s">
         <v>149</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -8818,7 +9335,7 @@
       <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96"/>
+      <c r="A3" s="95"/>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -8851,13 +9368,13 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="96"/>
+      <c r="A4" s="95"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="96"/>
+      <c r="A5" s="95"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -8899,7 +9416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8998,7 +9515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9034,7 +9551,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="88" t="s">
         <v>201</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -9060,7 +9577,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
@@ -9082,7 +9599,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -9104,7 +9621,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
@@ -9126,7 +9643,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="21" t="s">
         <v>1</v>
       </c>
@@ -9142,7 +9659,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="8" t="s">
         <v>151</v>
       </c>
@@ -9158,7 +9675,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
+      <c r="A8" s="88"/>
       <c r="B8" s="8" t="s">
         <v>152</v>
       </c>
@@ -9174,7 +9691,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="88"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -9184,7 +9701,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -9212,7 +9729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9236,7 +9753,7 @@
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="88" t="s">
         <v>209</v>
       </c>
       <c r="B2" s="8"/>
@@ -9248,7 +9765,7 @@
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -9258,7 +9775,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
@@ -9268,7 +9785,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="41"/>
@@ -9278,7 +9795,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -9288,7 +9805,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="8"/>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
@@ -9298,7 +9815,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
+      <c r="A8" s="88"/>
       <c r="B8" s="8"/>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -9308,7 +9825,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="88"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -9318,7 +9835,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -9346,7 +9863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9370,7 +9887,7 @@
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="88" t="s">
         <v>210</v>
       </c>
       <c r="B2" s="8"/>
@@ -9382,7 +9899,7 @@
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -9392,7 +9909,7 @@
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
@@ -9402,7 +9919,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="41"/>
@@ -9412,7 +9929,7 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -9422,7 +9939,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="8"/>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
@@ -9432,7 +9949,7 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
+      <c r="A8" s="88"/>
       <c r="B8" s="8"/>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -9442,7 +9959,7 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="88"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -9452,7 +9969,7 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="8"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>

</xml_diff>